<commit_message>
add deep learning - LSTM & CNN method
</commit_message>
<xml_diff>
--- a/allen/0314_allen.xlsx
+++ b/allen/0314_allen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allen/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allen/Documents/course/4490/Jan.29/allen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C183681-5F3F-C84F-BD11-73383045E36B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8D7F4B-8832-6147-87B2-631B3CB41584}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{AC1511F3-6BA7-BE48-A015-DD3B5079386A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="4" xr2:uid="{AC1511F3-6BA7-BE48-A015-DD3B5079386A}"/>
   </bookViews>
   <sheets>
     <sheet name="order diff_0.1" sheetId="1" r:id="rId1"/>
@@ -17600,8 +17600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF16A8E3-8919-453D-ABD1-0B00F4C48563}">
   <dimension ref="A1:AY53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y18" sqref="Y18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>

</xml_diff>